<commit_message>
added test type param to tests.m | Fixed stim and data path
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/tests/passed_tests.xlsx
+++ b/experiment/RUN_ME/tests/passed_tests.xlsx
@@ -1,26 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34FFF68-A8B7-4399-9991-1BBE790B0E64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -494,13 +484,13 @@
   </si>
   <si>
     <t xml:space="preserve">I ran these tests only once, and then changed the experiment's code a little bit.
-The output of the run is one of the files in development/data </t>
+The data i ran the tests on is in development/data </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,7 +704,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B9E31FB8-89B6-4315-BAB2-DE0E5FC682DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31FB8-89B6-4315-BAB2-DE0E5FC682DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -819,6 +809,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -854,6 +861,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1029,12 +1053,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>